<commit_message>
print total listening hours
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,56 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Taiwan thing after another: the Solomon Islands</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>00:20:44</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The Economist Asks: Eric Cantor</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>00:27:04</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Show currently playing episode
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,22 +462,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
+          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The first sentence of the story: Aung San Suu Kyi</t>
+          <t>The World Ahead: Year three</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:22:11</t>
+          <t>00:26:54</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
         </is>
       </c>
     </row>
@@ -487,22 +487,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
+          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Editor’s Picks: December 6th 2021</t>
+          <t>The first sentence of the story: Aung San Suu Kyi</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:23:40</t>
+          <t>00:22:11</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
         </is>
       </c>
     </row>
@@ -512,22 +512,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
+          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Checks and Balance: Courting controversy</t>
+          <t>Editor’s Picks: December 6th 2021</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:42:11</t>
+          <t>00:23:40</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
         </is>
       </c>
     </row>
@@ -537,22 +537,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
+          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Taiwan thing after another: the Solomon Islands</t>
+          <t>Checks and Balance: Courting controversy</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:20:44</t>
+          <t>00:42:11</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
         </is>
       </c>
     </row>
@@ -562,22 +562,97 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Taiwan thing after another: the Solomon Islands</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>00:20:44</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>The Economist Asks: Eric Cantor</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>00:27:04</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Roe blow? SCOTUS weighs abortion rights</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>00:24:02</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Wed, 01 Dec 2021 17:54:16 GMT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Money Talks: Omicronomics</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>00:31:01</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Show pretty terminal console
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,22 +462,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
+          <t>Tue, 07 Dec 2021 11:07:25 GMT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The World Ahead: Year three</t>
+          <t>Off the warpath: America 80 years after Pearl Harbour</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:26:54</t>
+          <t>00:22:48</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
         </is>
       </c>
     </row>
@@ -487,22 +487,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
+          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The first sentence of the story: Aung San Suu Kyi</t>
+          <t>The World Ahead: Year three</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:22:11</t>
+          <t>00:26:54</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
         </is>
       </c>
     </row>
@@ -512,22 +512,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
+          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Editor’s Picks: December 6th 2021</t>
+          <t>The first sentence of the story: Aung San Suu Kyi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:23:40</t>
+          <t>00:22:11</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
         </is>
       </c>
     </row>
@@ -537,22 +537,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
+          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Checks and Balance: Courting controversy</t>
+          <t>Editor’s Picks: December 6th 2021</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:42:11</t>
+          <t>00:23:40</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
         </is>
       </c>
     </row>
@@ -562,22 +562,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
+          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Taiwan thing after another: the Solomon Islands</t>
+          <t>Checks and Balance: Courting controversy</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:20:44</t>
+          <t>00:42:11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
         </is>
       </c>
     </row>
@@ -587,22 +587,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
+          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>The Economist Asks: Eric Cantor</t>
+          <t>Taiwan thing after another: the Solomon Islands</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:27:04</t>
+          <t>00:20:44</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
         </is>
       </c>
     </row>
@@ -612,22 +612,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
+          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Roe blow? SCOTUS weighs abortion rights</t>
+          <t>The Economist Asks: Eric Cantor</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>00:24:02</t>
+          <t>00:27:04</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
         </is>
       </c>
     </row>
@@ -637,20 +637,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Roe blow? SCOTUS weighs abortion rights</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>00:24:02</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Wed, 01 Dec 2021 17:54:16 GMT</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Money Talks: Omicronomics</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>00:31:01</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
         </is>

</xml_diff>

<commit_message>
Add the daily into my podcast player
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,247 +462,347 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tue, 07 Dec 2021 11:07:25 GMT</t>
+          <t>Tue, 7 Dec 2021 10:50:00 +0000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Off the warpath: America 80 years after Pearl Harbour</t>
+          <t>A New Strategy for Prosecuting School Shootings</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:22:48</t>
+          <t>00:23:29</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
+          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/e7d47081-01f3-426c-8f22-c117171ba5f5/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=e7d47081-01f3-426c-8f22-c117171ba5f5&amp;feed=54nAGcIl</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>1392</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
+          <t>Tue, 07 Dec 2021 11:07:25 GMT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The World Ahead: Year three</t>
+          <t>Off the warpath: America 80 years after Pearl Harbour</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:26:54</t>
+          <t>00:22:48</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>1393</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
+          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The first sentence of the story: Aung San Suu Kyi</t>
+          <t>The World Ahead: Year three</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:22:11</t>
+          <t>00:26:54</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>1394</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
+          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Editor’s Picks: December 6th 2021</t>
+          <t>The first sentence of the story: Aung San Suu Kyi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:23:40</t>
+          <t>00:22:11</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>1395</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
+          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Checks and Balance: Courting controversy</t>
+          <t>Editor’s Picks: December 6th 2021</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:42:11</t>
+          <t>00:23:40</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>1396</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
+          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Taiwan thing after another: the Solomon Islands</t>
+          <t>Checks and Balance: Courting controversy</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:20:44</t>
+          <t>00:42:11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>1397</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
+          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The Economist Asks: Eric Cantor</t>
+          <t>Taiwan thing after another: the Solomon Islands</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>00:27:04</t>
+          <t>00:20:44</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>1398</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
+          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Roe blow? SCOTUS weighs abortion rights</t>
+          <t>The Economist Asks: Eric Cantor</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:24:02</t>
+          <t>00:27:04</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>1399</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Wed, 01 Dec 2021 17:54:16 GMT</t>
+          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Money Talks: Omicronomics</t>
+          <t>Roe blow? SCOTUS weighs abortion rights</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>00:31:01</t>
+          <t>00:24:02</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>1400</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Wed, 01 Dec 2021 17:54:16 GMT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Money Talks: Omicronomics</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>00:31:01</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>1401</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>Wed, 01 Dec 2021 11:12:12 GMT</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>The house that Jack built: Twitter’s founder departs</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>00:19:35</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thehousethatjackbuilt-twitter-sfounderdeparts/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>1402</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Tue, 30 Nov 2021 18:05:41 GMT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Babbage: Omicron and on</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>00:28:32</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-omicronandon/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>1403</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Tue, 30 Nov 2021 10:57:53 GMT</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Centrifugal forces: Iran nuclear talks resume</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>00:22:51</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/centrifugalforces-irannucleartalksresume/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>1404</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mon, 29 Nov 2021 16:30:58 GMT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>The World Ahead: The eagle and the dragon</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>00:22:53</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-theeagleandthedragon/media.mp3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add The NPR Politics Podcast
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,324 +483,349 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1392</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tue, 07 Dec 2021 11:07:25 GMT</t>
+          <t>Mon, 6 Dec 2021 10:55:00 +0000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Off the warpath: America 80 years after Pearl Harbour</t>
+          <t>The Trial of Ghislaine Maxwell</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:22:48</t>
+          <t>00:32:59</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
+          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/4f9a4390-d07f-44dc-aabf-f87dece9fbd1/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=4f9a4390-d07f-44dc-aabf-f87dece9fbd1&amp;feed=54nAGcIl</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
+          <t>Tue, 07 Dec 2021 11:07:25 GMT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The World Ahead: Year three</t>
+          <t>Off the warpath: America 80 years after Pearl Harbour</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:26:54</t>
+          <t>00:22:48</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
+          <t>Mon, 06 Dec 2021 16:30:17 GMT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The first sentence of the story: Aung San Suu Kyi</t>
+          <t>The World Ahead: Year three</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:22:11</t>
+          <t>00:26:54</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
+          <t>Mon, 06 Dec 2021 11:14:06 GMT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Editor’s Picks: December 6th 2021</t>
+          <t>The first sentence of the story: Aung San Suu Kyi</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:23:40</t>
+          <t>00:22:11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
+          <t>Mon, 06 Dec 2021 00:01:00 GMT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Checks and Balance: Courting controversy</t>
+          <t>Editor’s Picks: December 6th 2021</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:42:11</t>
+          <t>00:23:40</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
+          <t>Fri, 03 Dec 2021 16:30:00 GMT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Taiwan thing after another: the Solomon Islands</t>
+          <t>Checks and Balance: Courting controversy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>00:20:44</t>
+          <t>00:42:11</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
+          <t>Fri, 03 Dec 2021 10:57:49 GMT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The Economist Asks: Eric Cantor</t>
+          <t>Taiwan thing after another: the Solomon Islands</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:27:04</t>
+          <t>00:20:44</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
+          <t>Thu, 02 Dec 2021 17:00:00 GMT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Roe blow? SCOTUS weighs abortion rights</t>
+          <t>The Economist Asks: Eric Cantor</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>00:24:02</t>
+          <t>00:27:04</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wed, 01 Dec 2021 17:54:16 GMT</t>
+          <t>Thu, 02 Dec 2021 11:05:06 GMT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Money Talks: Omicronomics</t>
+          <t>Roe blow? SCOTUS weighs abortion rights</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>00:31:01</t>
+          <t>00:24:02</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Wed, 01 Dec 2021 11:12:12 GMT</t>
+          <t>Wed, 01 Dec 2021 17:54:16 GMT</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The house that Jack built: Twitter’s founder departs</t>
+          <t>Money Talks: Omicronomics</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>00:19:35</t>
+          <t>00:31:01</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thehousethatjackbuilt-twitter-sfounderdeparts/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Tue, 30 Nov 2021 18:05:41 GMT</t>
+          <t>Wed, 01 Dec 2021 11:12:12 GMT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Babbage: Omicron and on</t>
+          <t>The house that Jack built: Twitter’s founder departs</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>00:28:32</t>
+          <t>00:19:35</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-omicronandon/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thehousethatjackbuilt-twitter-sfounderdeparts/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tue, 30 Nov 2021 10:57:53 GMT</t>
+          <t>Tue, 30 Nov 2021 18:05:41 GMT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Centrifugal forces: Iran nuclear talks resume</t>
+          <t>Babbage: Omicron and on</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>00:22:51</t>
+          <t>00:28:32</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/centrifugalforces-irannucleartalksresume/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-omicronandon/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
+        <v>1403</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Tue, 30 Nov 2021 10:57:53 GMT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Centrifugal forces: Iran nuclear talks resume</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>00:22:51</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/centrifugalforces-irannucleartalksresume/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>1404</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>Mon, 29 Nov 2021 16:30:58 GMT</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>The World Ahead: The eagle and the dragon</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>00:22:53</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-theeagleandthedragon/media.mp3</t>
         </is>

</xml_diff>

<commit_message>
Sort episodes by Published Date
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -508,7 +508,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1392</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -533,7 +533,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1393</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1394</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -583,7 +583,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1395</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1396</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1397</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -658,7 +658,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1398</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -683,7 +683,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1399</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1400</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -733,7 +733,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1401</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -758,7 +758,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1402</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1403</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -808,7 +808,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>1404</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add more podcast channels
</commit_message>
<xml_diff>
--- a/played_theeconomist.xlsx
+++ b/played_theeconomist.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,505 +508,551 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44537</v>
+        <v>44538</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Why Women Seek Abortions After 15 Weeks</t>
+          <t>推特迎新掌门人，印度为何「盛产」硅谷 CEO ？</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>855</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211207_nprpolitics_120721politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1062189783&amp;orgId=1&amp;d=855&amp;p=510310&amp;story=1062189783&amp;t=podcast&amp;e=1062189783&amp;size=13693223&amp;ft=pod&amp;f=510310</t>
+          <t>https://aphid.fireside.fm/d/1437767933/12647593-905b-40ef-8977-371837f74e89/495fb43c-6a24-4b2d-a148-9f8291116987.mp3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>44537</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Babbage: Goodbye darkness, my old friend</t>
+          <t>Why Women Seek Abortions After 15 Weeks</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:29:19</t>
+          <t>855</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-goodbyedarkness-myoldfriend/media.mp3</t>
+          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211207_nprpolitics_120721politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1062189783&amp;orgId=1&amp;d=855&amp;p=510310&amp;story=1062189783&amp;t=podcast&amp;e=1062189783&amp;size=13693223&amp;ft=pod&amp;f=510310</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>44537</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Off the warpath: America 80 years after Pearl Harbour</t>
+          <t>Babbage: Goodbye darkness, my old friend</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:22:48</t>
+          <t>00:29:19</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-goodbyedarkness-myoldfriend/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>44537</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A New Strategy for Prosecuting School Shootings</t>
+          <t>Off the warpath: America 80 years after Pearl Harbour</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:23:29</t>
+          <t>00:22:48</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/e7d47081-01f3-426c-8f22-c117171ba5f5/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=e7d47081-01f3-426c-8f22-c117171ba5f5&amp;feed=54nAGcIl</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/offthewarpath-america80yearsafterpearlharbour/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44536</v>
+        <v>44537</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The High Cost Of Vaccine Conspiracies</t>
+          <t>A New Strategy for Prosecuting School Shootings</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>925</t>
+          <t>00:23:29</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211206_nprpolitics_120621politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1061893017&amp;orgId=1&amp;d=925&amp;p=510310&amp;story=1061893017&amp;t=podcast&amp;e=1061893017&amp;size=14810846&amp;ft=pod&amp;f=510310</t>
+          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/e7d47081-01f3-426c-8f22-c117171ba5f5/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=e7d47081-01f3-426c-8f22-c117171ba5f5&amp;feed=54nAGcIl</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>44536</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The World Ahead: Year three</t>
+          <t>The High Cost Of Vaccine Conspiracies</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:26:54</t>
+          <t>925</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
+          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211206_nprpolitics_120621politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1061893017&amp;orgId=1&amp;d=925&amp;p=510310&amp;story=1061893017&amp;t=podcast&amp;e=1061893017&amp;size=14810846&amp;ft=pod&amp;f=510310</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>44536</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>The first sentence of the story: Aung San Suu Kyi</t>
+          <t>The World Ahead: Year three</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>00:22:11</t>
+          <t>00:26:54</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-yearthree/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>44536</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>The Trial of Ghislaine Maxwell</t>
+          <t>The first sentence of the story: Aung San Suu Kyi</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>00:32:59</t>
+          <t>00:22:11</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/4f9a4390-d07f-44dc-aabf-f87dece9fbd1/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=4f9a4390-d07f-44dc-aabf-f87dece9fbd1&amp;feed=54nAGcIl</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thefirstsentenceofthestory-aungsansuukyi/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>44536</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Editor’s Picks: December 6th 2021</t>
+          <t>The Trial of Ghislaine Maxwell</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>00:23:40</t>
+          <t>00:32:59</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
+          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/4f9a4390-d07f-44dc-aabf-f87dece9fbd1/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=4f9a4390-d07f-44dc-aabf-f87dece9fbd1&amp;feed=54nAGcIl</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44535</v>
+        <v>44536</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The Sunday Read: ‘The Emily Ratajkowski You’ll Never See’</t>
+          <t>Editor’s Picks: December 6th 2021</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>00:37:28</t>
+          <t>00:23:40</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/105376fb-f573-4b62-ac4d-a8adfa84ae88/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=105376fb-f573-4b62-ac4d-a8adfa84ae88&amp;feed=54nAGcIl</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomisteditorspicks/editor-spicks-december6th2021/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44533</v>
+        <v>44535</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Weekly Roundup: December 3rd</t>
+          <t>The Sunday Read: ‘The Emily Ratajkowski You’ll Never See’</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1494</t>
+          <t>00:37:28</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211203_nprpolitics_120321politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1061326912&amp;orgId=1&amp;d=1494&amp;p=510310&amp;story=1061326912&amp;t=podcast&amp;e=1061326912&amp;size=23918177&amp;ft=pod&amp;f=510310</t>
+          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/105376fb-f573-4b62-ac4d-a8adfa84ae88/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=105376fb-f573-4b62-ac4d-a8adfa84ae88&amp;feed=54nAGcIl</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>44533</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Checks and Balance: Courting controversy</t>
+          <t>Weekly Roundup: December 3rd</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>00:42:11</t>
+          <t>1494</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
+          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211203_nprpolitics_120321politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1061326912&amp;orgId=1&amp;d=1494&amp;p=510310&amp;story=1061326912&amp;t=podcast&amp;e=1061326912&amp;size=23918177&amp;ft=pod&amp;f=510310</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>44533</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Taiwan thing after another: the Solomon Islands</t>
+          <t>Checks and Balance: Courting controversy</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>00:20:44</t>
+          <t>00:42:11</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/checksandbalance/checksandbalance-courtingcontroversy/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>44533</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>The Life and Legacy of Stephen Sondheim</t>
+          <t>Taiwan thing after another: the Solomon Islands</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>00:34:32</t>
+          <t>00:20:44</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/049bb822-b8d7-4e29-86b3-77328022101f/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=049bb822-b8d7-4e29-86b3-77328022101f&amp;feed=54nAGcIl</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/taiwanthingafteranother-thesolomonislands/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44532</v>
+        <v>44533</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Why Two Experts Think The Supreme Court Is Prepared To Roll Back Roe V. Wade</t>
+          <t>The Life and Legacy of Stephen Sondheim</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>00:34:32</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211202_nprpolitics_120221politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1061044346&amp;orgId=1&amp;d=832&amp;p=510310&amp;story=1061044346&amp;t=podcast&amp;e=1061044346&amp;size=13321658&amp;ft=pod&amp;f=510310</t>
+          <t>https://dts.podtrac.com/redirect.mp3/chrt.fm/track/8DB4DB/pdst.fm/e/nyt.simplecastaudio.com/03d8b493-87fc-4bd1-931f-8a8e9b945d8a/episodes/049bb822-b8d7-4e29-86b3-77328022101f/audio/128/default.mp3?aid=rss_feed&amp;awCollectionId=03d8b493-87fc-4bd1-931f-8a8e9b945d8a&amp;awEpisodeId=049bb822-b8d7-4e29-86b3-77328022101f&amp;feed=54nAGcIl</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>44532</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>The Economist Asks: Eric Cantor</t>
+          <t>Why Two Experts Think The Supreme Court Is Prepared To Roll Back Roe V. Wade</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>00:27:04</t>
+          <t>832</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
+          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211202_nprpolitics_120221politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1061044346&amp;orgId=1&amp;d=832&amp;p=510310&amp;story=1061044346&amp;t=podcast&amp;e=1061044346&amp;size=13321658&amp;ft=pod&amp;f=510310</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>44532</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Roe blow? SCOTUS weighs abortion rights</t>
+          <t>The Economist Asks: Eric Cantor</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>00:24:02</t>
+          <t>00:27:04</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistasks/theeconomistasks-ericcantor/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44531</v>
+        <v>44532</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Money Talks: Omicronomics</t>
+          <t>Roe blow? SCOTUS weighs abortion rights</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>00:31:01</t>
+          <t>00:24:02</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/roeblow-scotusweighsabortionrights/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>44531</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>The house that Jack built: Twitter’s founder departs</t>
+          <t>The Big Consequences Of Small Changes To Congressional Maps</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>00:19:35</t>
+          <t>894</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thehousethatjackbuilt-twitter-sfounderdeparts/media.mp3</t>
+          <t>https://play.podtrac.com/npr-510310/edge1.pod.npr.org/anon.npr-mp3/npr/nprpolitics/2021/12/20211201_nprpolitics_120121politicspodcast.mp3?awCollectionId=510310&amp;awEpisodeId=1060610347&amp;orgId=1&amp;d=894&amp;p=510310&amp;story=1060610347&amp;t=podcast&amp;e=1060610347&amp;size=14304698&amp;ft=pod&amp;f=510310</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44530</v>
+        <v>44531</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Babbage: Omicron and on</t>
+          <t>Money Talks: Omicronomics</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>00:28:32</t>
+          <t>00:31:01</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-omicronandon/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistmoneytalks/moneytalks-omicronomics/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44530</v>
+        <v>44531</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Centrifugal forces: Iran nuclear talks resume</t>
+          <t>The house that Jack built: Twitter’s founder departs</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>00:22:51</t>
+          <t>00:19:35</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/centrifugalforces-irannucleartalksresume/media.mp3</t>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/thehousethatjackbuilt-twitter-sfounderdeparts/media.mp3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Babbage: Omicron and on</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>00:28:32</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theeconomistbabbage/babbage-omicronandon/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Centrifugal forces: Iran nuclear talks resume</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>00:22:51</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://sphinx.acast.com/theeconomistallaudio/theintelligencepodcast/centrifugalforces-irannucleartalksresume/media.mp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B27" s="2" t="n">
         <v>44529</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>The World Ahead: The eagle and the dragon</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>00:22:53</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>https://sphinx.acast.com/theeconomistallaudio/theworldahead/theworldahead-theeagleandthedragon/media.mp3</t>
         </is>

</xml_diff>